<commit_message>
Pulled latest survey responses from Google forms and removed our test cases
</commit_message>
<xml_diff>
--- a/survey_responses.xlsx
+++ b/survey_responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorensabet/Desktop/MSC/CSC2506_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F3F527-6999-4C43-B37C-E558DD45A3F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367797CC-5AA2-3946-B1A4-268F6490B949}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{80281BEE-6CAF-E644-99B3-D2BCEA94F5D9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="78">
   <si>
     <t>Please enter your name</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>4/16/2021 16:27:56</t>
+  </si>
+  <si>
+    <t>4/17/2021 14:14:25</t>
+  </si>
+  <si>
+    <t>4/17/2021 15:02:26</t>
+  </si>
+  <si>
+    <t>4/17/2021 15:50:31</t>
   </si>
 </sst>
 </file>
@@ -617,10 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D43AA-5323-EA46-9B61-4F0E168AEE91}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3919,6 +3929,168 @@
         <v>2</v>
       </c>
     </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="1">
+        <v>3</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K62" s="1">
+        <v>2</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M62" s="1">
+        <v>1</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P62" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>2</v>
+      </c>
+      <c r="R62" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="1">
+        <v>3</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K63" s="1">
+        <v>3</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M63" s="1">
+        <v>1</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O63" s="1">
+        <v>2</v>
+      </c>
+      <c r="P63" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="1">
+        <v>5</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="1">
+        <v>5</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64" s="1">
+        <v>5</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" s="1">
+        <v>5</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M64" s="1">
+        <v>5</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>